<commit_message>
heaps of new tests and nice diagrams for the random fererst :)
</commit_message>
<xml_diff>
--- a/Code/Ferns/Random Ferns/Evaluation/Evaluation.xlsx
+++ b/Code/Ferns/Random Ferns/Evaluation/Evaluation.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Times</t>
   </si>
@@ -27,10 +27,16 @@
     <t>(#Ferns = 1)</t>
   </si>
   <si>
-    <t>Size/depth of Fern:</t>
+    <t>Time for Evaluation:</t>
   </si>
   <si>
-    <t>Time for Evaluation:</t>
+    <t>Depth of Fern:</t>
+  </si>
+  <si>
+    <t>Accuracy on Valid:</t>
+  </si>
+  <si>
+    <t>Accuracy on Train:</t>
   </si>
 </sst>
 </file>
@@ -61,7 +67,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -108,16 +114,112 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -130,6 +232,776 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy on Train:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$12:$AA$12</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.38182262753230756</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.3059869773507331</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38071778524401617</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17887577769124186</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33069197540367495</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16453094011211433</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30662090325385111</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47011039366798585</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.69067132753140192</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.56641279443594184</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.53274227289604525</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.38975575740561297</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.42192296894668685</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.62636407270224503</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.56510871829238474</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.6289178884833776</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66930802459632499</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.47641342836184492</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.55954828251360678</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65265388551298187</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.72815446057433686</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.68717567897992271</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.45347436675330322</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.62928013185658782</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68452224627115732</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy on Valid:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$13:$AA$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0.38107226951639195</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.30601340336895488</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.38040210106864697</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.17884441224415867</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33184205759826119</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.16301394674877739</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.30507154500996198</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.47141822133671435</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.68764716536859261</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.5655316065930085</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.5318420575982612</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.38715812352834633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.42211555877558415</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.62885346857453361</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.56297772142727764</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.62798406085854008</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.66766890056149253</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.47609128781017934</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.55951820322405366</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.65051621083137112</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.72836442673428725</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.6859808005796052</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.45165730845861257</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.62791161021554065</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.68136207208838995</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="52114944"/>
+        <c:axId val="41431552"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="52114944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="41431552"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="41431552"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="52114944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$8</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time for Training:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$8:$AB$8</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>8.401437727351464</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.555468303917984</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>14.173659628795606</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>19.173648080784751</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20.248054480948991</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>22.801286320098029</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>25.341352785316062</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28.439567334526629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>31.462372089740875</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>34.578055571594462</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>37.544083248327141</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>54.269191831706991</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>43.844225673794355</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>55.195219765062134</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>72.06777078481565</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>60.637028696806972</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73.321679465712037</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>70.712208172142354</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>101.78265617080791</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>91.914672389347601</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>115.26079129536603</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>158.81196438080207</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>236.41935703241782</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>471.34704402999915</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>739.11075055654999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>1618.6778291022704</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="88837632"/>
+        <c:axId val="167375936"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88837632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="167375936"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="167375936"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88837632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Tabelle1!$B$9</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time for Evaluation:</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Tabelle1!$C$9:$AA$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>4.1829461541916099E-4</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.24173937901047E-4</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.931911644885835E-4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.1252060999159563E-4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.5165553566731462E-4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.6697012272969315E-4</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.5045518409453968E-4</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.3377472397046278E-4</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>7.3650647009385962E-4</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>4.8373334359823187E-4</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.7106774191478852E-4</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.3923821621725656E-4</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>6.184601369080843E-4</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.9031442667333884E-4</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.0001860512859992E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.0138640285877423E-4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.2657903009539941E-3</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.1881620057611743E-3</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.3658730616984557E-3</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.3042836704710947E-3</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.2779798679677427E-3</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.3921768642018079E-3</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>1.3761379602363494E-3</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.0311667981856791E-3</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.7103887188765069E-3</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="88948736"/>
+        <c:axId val="134677632"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="88948736"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="134677632"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="134677632"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="88948736"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.78740157499999996" l="0.7" r="0.7" t="0.78740157499999996" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Diagramm 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266699</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>166686</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagramm 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>176211</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>504825</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Diagramm 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -419,10 +1291,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:Q9"/>
+  <dimension ref="B3:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V10" sqref="V10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -430,21 +1302,21 @@
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:17" ht="46.5" x14ac:dyDescent="0.7">
+    <row r="3" spans="2:28" ht="46.5" x14ac:dyDescent="0.7">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="2">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
         <v>1</v>
       </c>
       <c r="D7" s="2">
@@ -486,53 +1358,373 @@
       <c r="P7" s="2">
         <v>14</v>
       </c>
-      <c r="Q7" s="3">
+      <c r="Q7" s="2">
         <v>15</v>
       </c>
+      <c r="R7" s="2">
+        <v>16</v>
+      </c>
+      <c r="S7" s="2">
+        <v>17</v>
+      </c>
+      <c r="T7" s="2">
+        <v>18</v>
+      </c>
+      <c r="U7" s="2">
+        <v>19</v>
+      </c>
+      <c r="V7" s="2">
+        <v>20</v>
+      </c>
+      <c r="W7" s="2">
+        <v>21</v>
+      </c>
+      <c r="X7" s="2">
+        <v>22</v>
+      </c>
+      <c r="Y7" s="2">
+        <v>23</v>
+      </c>
+      <c r="Z7" s="2">
+        <v>24</v>
+      </c>
+      <c r="AA7" s="2">
+        <v>25</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>26</v>
+      </c>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
-      <c r="N8" s="2"/>
-      <c r="O8" s="2"/>
-      <c r="P8" s="2"/>
-      <c r="Q8" s="3"/>
+      <c r="C8" s="6">
+        <v>8.401437727351464</v>
+      </c>
+      <c r="D8" s="7">
+        <v>18.555468303917984</v>
+      </c>
+      <c r="E8" s="7">
+        <v>14.173659628795606</v>
+      </c>
+      <c r="F8" s="7">
+        <v>19.173648080784751</v>
+      </c>
+      <c r="G8" s="7">
+        <v>20.248054480948991</v>
+      </c>
+      <c r="H8" s="7">
+        <v>22.801286320098029</v>
+      </c>
+      <c r="I8" s="7">
+        <v>25.341352785316062</v>
+      </c>
+      <c r="J8" s="7">
+        <v>28.439567334526629</v>
+      </c>
+      <c r="K8" s="7">
+        <v>31.462372089740875</v>
+      </c>
+      <c r="L8" s="7">
+        <v>34.578055571594462</v>
+      </c>
+      <c r="M8" s="7">
+        <v>37.544083248327141</v>
+      </c>
+      <c r="N8" s="7">
+        <v>54.269191831706991</v>
+      </c>
+      <c r="O8" s="7">
+        <v>43.844225673794355</v>
+      </c>
+      <c r="P8" s="7">
+        <v>55.195219765062134</v>
+      </c>
+      <c r="Q8" s="7">
+        <v>72.06777078481565</v>
+      </c>
+      <c r="R8" s="7">
+        <v>60.637028696806972</v>
+      </c>
+      <c r="S8" s="7">
+        <v>73.321679465712037</v>
+      </c>
+      <c r="T8" s="7">
+        <v>70.712208172142354</v>
+      </c>
+      <c r="U8" s="7">
+        <v>101.78265617080791</v>
+      </c>
+      <c r="V8" s="7">
+        <v>91.914672389347601</v>
+      </c>
+      <c r="W8" s="7">
+        <v>115.26079129536603</v>
+      </c>
+      <c r="X8" s="7">
+        <v>158.81196438080207</v>
+      </c>
+      <c r="Y8" s="7">
+        <v>236.41935703241782</v>
+      </c>
+      <c r="Z8" s="7">
+        <v>471.34704402999915</v>
+      </c>
+      <c r="AA8" s="7">
+        <v>739.11075055654999</v>
+      </c>
+      <c r="AB8" s="8">
+        <v>1618.6778291022704</v>
+      </c>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
-      <c r="N9" s="2"/>
-      <c r="O9" s="2"/>
-      <c r="P9" s="2"/>
-      <c r="Q9" s="3"/>
+        <v>3</v>
+      </c>
+      <c r="C9" s="9">
+        <v>4.1829461541916099E-4</v>
+      </c>
+      <c r="D9" s="10">
+        <v>3.24173937901047E-4</v>
+      </c>
+      <c r="E9" s="10">
+        <v>2.931911644885835E-4</v>
+      </c>
+      <c r="F9" s="10">
+        <v>4.1252060999159563E-4</v>
+      </c>
+      <c r="G9" s="10">
+        <v>4.5165553566731462E-4</v>
+      </c>
+      <c r="H9" s="10">
+        <v>3.6697012272969315E-4</v>
+      </c>
+      <c r="I9" s="10">
+        <v>5.5045518409453968E-4</v>
+      </c>
+      <c r="J9" s="10">
+        <v>5.3377472397046278E-4</v>
+      </c>
+      <c r="K9" s="10">
+        <v>7.3650647009385962E-4</v>
+      </c>
+      <c r="L9" s="10">
+        <v>4.8373334359823187E-4</v>
+      </c>
+      <c r="M9" s="10">
+        <v>6.7106774191478852E-4</v>
+      </c>
+      <c r="N9" s="10">
+        <v>9.3923821621725656E-4</v>
+      </c>
+      <c r="O9" s="10">
+        <v>6.184601369080843E-4</v>
+      </c>
+      <c r="P9" s="10">
+        <v>6.9031442667333884E-4</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>1.0001860512859992E-3</v>
+      </c>
+      <c r="R9" s="10">
+        <v>9.0138640285877423E-4</v>
+      </c>
+      <c r="S9" s="10">
+        <v>1.2657903009539941E-3</v>
+      </c>
+      <c r="T9" s="10">
+        <v>1.1881620057611743E-3</v>
+      </c>
+      <c r="U9" s="10">
+        <v>1.3658730616984557E-3</v>
+      </c>
+      <c r="V9" s="10">
+        <v>1.3042836704710947E-3</v>
+      </c>
+      <c r="W9" s="10">
+        <v>1.2779798679677427E-3</v>
+      </c>
+      <c r="X9" s="10">
+        <v>1.3921768642018079E-3</v>
+      </c>
+      <c r="Y9" s="10">
+        <v>1.3761379602363494E-3</v>
+      </c>
+      <c r="Z9" s="10">
+        <v>2.0311667981856791E-3</v>
+      </c>
+      <c r="AA9" s="10">
+        <v>1.7103887188765069E-3</v>
+      </c>
+      <c r="AB9" s="11"/>
+    </row>
+    <row r="12" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6">
+        <v>0.38182262753230756</v>
+      </c>
+      <c r="D12" s="7">
+        <v>0.3059869773507331</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0.38071778524401617</v>
+      </c>
+      <c r="F12" s="7">
+        <v>0.17887577769124186</v>
+      </c>
+      <c r="G12" s="7">
+        <v>0.33069197540367495</v>
+      </c>
+      <c r="H12" s="7">
+        <v>0.16453094011211433</v>
+      </c>
+      <c r="I12" s="7">
+        <v>0.30662090325385111</v>
+      </c>
+      <c r="J12" s="7">
+        <v>0.47011039366798585</v>
+      </c>
+      <c r="K12" s="7">
+        <v>0.69067132753140192</v>
+      </c>
+      <c r="L12" s="7">
+        <v>0.56641279443594184</v>
+      </c>
+      <c r="M12" s="7">
+        <v>0.53274227289604525</v>
+      </c>
+      <c r="N12" s="7">
+        <v>0.38975575740561297</v>
+      </c>
+      <c r="O12" s="7">
+        <v>0.42192296894668685</v>
+      </c>
+      <c r="P12" s="7">
+        <v>0.62636407270224503</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>0.56510871829238474</v>
+      </c>
+      <c r="R12" s="7">
+        <v>0.6289178884833776</v>
+      </c>
+      <c r="S12" s="7">
+        <v>0.66930802459632499</v>
+      </c>
+      <c r="T12" s="7">
+        <v>0.47641342836184492</v>
+      </c>
+      <c r="U12" s="7">
+        <v>0.55954828251360678</v>
+      </c>
+      <c r="V12" s="7">
+        <v>0.65265388551298187</v>
+      </c>
+      <c r="W12" s="7">
+        <v>0.72815446057433686</v>
+      </c>
+      <c r="X12" s="7">
+        <v>0.68717567897992271</v>
+      </c>
+      <c r="Y12" s="7">
+        <v>0.45347436675330322</v>
+      </c>
+      <c r="Z12" s="7">
+        <v>0.62928013185658782</v>
+      </c>
+      <c r="AA12" s="7">
+        <v>0.68452224627115732</v>
+      </c>
+      <c r="AB12" s="8"/>
+    </row>
+    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.38107226951639195</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.30601340336895488</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.38040210106864697</v>
+      </c>
+      <c r="F13" s="10">
+        <v>0.17884441224415867</v>
+      </c>
+      <c r="G13" s="10">
+        <v>0.33184205759826119</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.16301394674877739</v>
+      </c>
+      <c r="I13" s="10">
+        <v>0.30507154500996198</v>
+      </c>
+      <c r="J13" s="10">
+        <v>0.47141822133671435</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.68764716536859261</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0.5655316065930085</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0.5318420575982612</v>
+      </c>
+      <c r="N13" s="10">
+        <v>0.38715812352834633</v>
+      </c>
+      <c r="O13" s="10">
+        <v>0.42211555877558415</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0.62885346857453361</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0.56297772142727764</v>
+      </c>
+      <c r="R13" s="10">
+        <v>0.62798406085854008</v>
+      </c>
+      <c r="S13" s="10">
+        <v>0.66766890056149253</v>
+      </c>
+      <c r="T13" s="10">
+        <v>0.47609128781017934</v>
+      </c>
+      <c r="U13" s="10">
+        <v>0.55951820322405366</v>
+      </c>
+      <c r="V13" s="10">
+        <v>0.65051621083137112</v>
+      </c>
+      <c r="W13" s="10">
+        <v>0.72836442673428725</v>
+      </c>
+      <c r="X13" s="10">
+        <v>0.6859808005796052</v>
+      </c>
+      <c r="Y13" s="10">
+        <v>0.45165730845861257</v>
+      </c>
+      <c r="Z13" s="10">
+        <v>0.62791161021554065</v>
+      </c>
+      <c r="AA13" s="10">
+        <v>0.68136207208838995</v>
+      </c>
+      <c r="AB13" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added last content for Fern Testing and the Results - Comparison section. Proof-read by Jonas :)
</commit_message>
<xml_diff>
--- a/Code/Ferns/Random Ferns/Evaluation/Evaluation.xlsx
+++ b/Code/Ferns/Random Ferns/Evaluation/Evaluation.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="165" windowWidth="14805" windowHeight="7950"/>
+    <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
     <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
     <sheet name="Tabelle3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
@@ -240,7 +240,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -473,11 +473,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54337536"/>
-        <c:axId val="54339072"/>
+        <c:axId val="42092032"/>
+        <c:axId val="72976064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54337536"/>
+        <c:axId val="42092032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -486,7 +486,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54339072"/>
+        <c:crossAx val="72976064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -494,7 +494,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54339072"/>
+        <c:axId val="72976064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -505,7 +505,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54337536"/>
+        <c:crossAx val="42092032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -530,7 +530,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -667,11 +667,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54367744"/>
-        <c:axId val="54369280"/>
+        <c:axId val="42093056"/>
+        <c:axId val="72977792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54367744"/>
+        <c:axId val="42093056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -680,7 +680,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54369280"/>
+        <c:crossAx val="72977792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -688,7 +688,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="54369280"/>
+        <c:axId val="72977792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -699,7 +699,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54367744"/>
+        <c:crossAx val="42093056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -724,7 +724,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -858,11 +858,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="54381952"/>
-        <c:axId val="52569216"/>
+        <c:axId val="42093568"/>
+        <c:axId val="72979520"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="54381952"/>
+        <c:axId val="42093568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -871,7 +871,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52569216"/>
+        <c:crossAx val="72979520"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -879,7 +879,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52569216"/>
+        <c:axId val="72979520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -890,7 +890,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="54381952"/>
+        <c:crossAx val="42093568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -915,7 +915,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-GB"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1028,11 +1028,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="52597888"/>
-        <c:axId val="52599424"/>
+        <c:axId val="42094080"/>
+        <c:axId val="72981248"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="52597888"/>
+        <c:axId val="42094080"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1041,7 +1041,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52599424"/>
+        <c:crossAx val="72981248"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1049,7 +1049,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52599424"/>
+        <c:axId val="72981248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1060,7 +1060,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52597888"/>
+        <c:crossAx val="42094080"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1496,7 +1496,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:AB13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>

</xml_diff>